<commit_message>
calorimetry : tests : regression tests : WIP
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.1.dsc/data.xlsx
+++ b/output/calorimetry/ds.1.dsc/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">PLP</t>
   </si>
@@ -61,25 +61,28 @@
     <t xml:space="preserve">res.rel</t>
   </si>
   <si>
-    <t xml:space="preserve">cnst</t>
+    <t xml:space="preserve">Constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St.Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
   <si>
     <t xml:space="preserve">dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -1109,15 +1112,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1125,7 +1128,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1133,10 +1136,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1730,7 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -1804,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1856,10 +1859,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -1872,130 +1875,130 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2017,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
calorimetry : input and output consistency : WIP
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.1.dsc/data.xlsx
+++ b/output/calorimetry/ds.1.dsc/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t xml:space="preserve">PLP</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">res.rel</t>
   </si>
   <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
     <t xml:space="preserve">Constant</t>
   </si>
   <si>
@@ -70,9 +73,18 @@
     <t xml:space="preserve">Validity</t>
   </si>
   <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">OK</t>
   </si>
   <si>
+    <t xml:space="preserve">5.12441253662109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0266629716825117</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
@@ -86,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">tot</t>
@@ -1074,10 +1089,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -1112,15 +1127,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1128,7 +1143,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1136,10 +1151,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1644,38 +1659,50 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>5.12441253662109</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0266629716825117</v>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1721,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1724,13 +1751,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
@@ -1807,39 +1834,17 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1859,10 +1864,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -1875,130 +1880,130 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2022,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
calorimetry : new datasets : WIP
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.1.dsc/data.xlsx
+++ b/output/calorimetry/ds.1.dsc/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">PLP</t>
   </si>
@@ -73,12 +73,6 @@
     <t xml:space="preserve">Validity</t>
   </si>
   <si>
-    <t xml:space="preserve">5.12441253662109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0266629716825117</t>
-  </si>
-  <si>
     <t xml:space="preserve">OK</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">tot</t>
@@ -1086,22 +1077,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1120,15 +1099,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1136,7 +1115,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1144,10 +1123,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1660,14 +1639,14 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="n">
+        <v>5.12441253662109</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0266629716825117</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1686,7 +1665,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1716,13 +1695,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -1777,15 +1756,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1807,10 +1786,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -1823,130 +1802,130 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1965,7 +1944,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">

</xml_diff>